<commit_message>
Update and sort the BOM file
</commit_message>
<xml_diff>
--- a/HACKberry_BOM_v2.xlsx
+++ b/HACKberry_BOM_v2.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Full kit" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Full kit'!$A$1:$H$97</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Full kit'!$A$1:$H$100</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="258">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -1074,6 +1074,34 @@
   </si>
   <si>
     <t>R-W-03.stl (or L-W-03.stl)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>External Battery</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C-B-01.stl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C-B-02.stl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C-B-03.stl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3D print part (old name: HbBatteryLockKnob01.stl)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3D print part (old name: HbBatteryCase01.stl)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3D print part (old name: HbBatteryCaseHolder01.stl)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1257,6 +1285,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1265,15 +1302,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1580,11 +1608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
@@ -1871,10 +1899,10 @@
         <v>129</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1887,10 +1915,10 @@
     <row r="18" spans="1:8">
       <c r="A18" s="16"/>
       <c r="B18" s="2" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1903,10 +1931,10 @@
     <row r="19" spans="1:8">
       <c r="A19" s="16"/>
       <c r="B19" s="2" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1919,10 +1947,10 @@
     <row r="20" spans="1:8">
       <c r="A20" s="16"/>
       <c r="B20" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1935,10 +1963,10 @@
     <row r="21" spans="1:8">
       <c r="A21" s="16"/>
       <c r="B21" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1951,10 +1979,10 @@
     <row r="22" spans="1:8">
       <c r="A22" s="16"/>
       <c r="B22" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -1967,10 +1995,10 @@
     <row r="23" spans="1:8">
       <c r="A23" s="16"/>
       <c r="B23" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -1983,10 +2011,10 @@
     <row r="24" spans="1:8">
       <c r="A24" s="16"/>
       <c r="B24" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -1999,10 +2027,10 @@
     <row r="25" spans="1:8">
       <c r="A25" s="16"/>
       <c r="B25" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -2015,10 +2043,10 @@
     <row r="26" spans="1:8">
       <c r="A26" s="17"/>
       <c r="B26" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -2033,10 +2061,10 @@
         <v>128</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -2081,10 +2109,10 @@
     <row r="30" spans="1:8">
       <c r="A30" s="16"/>
       <c r="B30" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
@@ -2097,10 +2125,10 @@
     <row r="31" spans="1:8">
       <c r="A31" s="16"/>
       <c r="B31" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -2113,10 +2141,10 @@
     <row r="32" spans="1:8">
       <c r="A32" s="16"/>
       <c r="B32" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
@@ -2129,10 +2157,10 @@
     <row r="33" spans="1:8">
       <c r="A33" s="16"/>
       <c r="B33" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D33" s="2">
         <v>1</v>
@@ -2143,14 +2171,14 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="18" t="s">
         <v>86</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
@@ -2161,7 +2189,7 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="2" t="s">
         <v>232</v>
       </c>
@@ -2177,12 +2205,12 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D36" s="2">
         <v>3</v>
@@ -2193,12 +2221,12 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="22"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D37" s="2">
         <v>3</v>
@@ -2209,12 +2237,12 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="23"/>
+      <c r="A38" s="20"/>
       <c r="B38" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D38" s="2">
         <v>3</v>
@@ -2229,10 +2257,10 @@
         <v>131</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D39" s="2">
         <v>1</v>
@@ -2245,10 +2273,10 @@
     <row r="40" spans="1:8">
       <c r="A40" s="17"/>
       <c r="B40" s="2" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -2260,13 +2288,13 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="15" t="s">
-        <v>132</v>
+        <v>251</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -2279,10 +2307,10 @@
     <row r="42" spans="1:8">
       <c r="A42" s="16"/>
       <c r="B42" s="2" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>201</v>
+        <v>255</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -2293,12 +2321,12 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="2" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>202</v>
+        <v>256</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
@@ -2309,12 +2337,14 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="16"/>
+      <c r="A44" s="15" t="s">
+        <v>132</v>
+      </c>
       <c r="B44" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
@@ -2327,10 +2357,10 @@
     <row r="45" spans="1:8">
       <c r="A45" s="16"/>
       <c r="B45" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D45" s="2">
         <v>1</v>
@@ -2341,12 +2371,12 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D46" s="2">
         <v>1</v>
@@ -2357,14 +2387,12 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="15" t="s">
-        <v>133</v>
-      </c>
+      <c r="A47" s="16"/>
       <c r="B47" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D47" s="2">
         <v>1</v>
@@ -2377,10 +2405,10 @@
     <row r="48" spans="1:8">
       <c r="A48" s="16"/>
       <c r="B48" s="2" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="D48" s="2">
         <v>1</v>
@@ -2391,12 +2419,12 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="16"/>
+      <c r="A49" s="17"/>
       <c r="B49" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
@@ -2407,12 +2435,14 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="16"/>
+      <c r="A50" s="15" t="s">
+        <v>133</v>
+      </c>
       <c r="B50" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D50" s="2">
         <v>1</v>
@@ -2425,10 +2455,10 @@
     <row r="51" spans="1:8">
       <c r="A51" s="16"/>
       <c r="B51" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
@@ -2441,10 +2471,10 @@
     <row r="52" spans="1:8">
       <c r="A52" s="16"/>
       <c r="B52" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
@@ -2457,10 +2487,10 @@
     <row r="53" spans="1:8">
       <c r="A53" s="16"/>
       <c r="B53" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
@@ -2472,922 +2502,971 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="16"/>
-      <c r="B54" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="D54" s="7">
-        <v>1</v>
-      </c>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
+      <c r="B54" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="16"/>
+      <c r="B56" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="16"/>
+      <c r="B57" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="7">
+        <v>1</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B59" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C59" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="D56" s="8">
-        <v>1</v>
-      </c>
-      <c r="E56" s="9" t="s">
+      <c r="D59" s="8">
+        <v>1</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="9" t="s">
+      <c r="F59" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G59" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H59" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="93.75">
-      <c r="A57" s="16"/>
-      <c r="B57" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="2">
-        <v>6</v>
-      </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" ht="75">
-      <c r="A58" s="16"/>
-      <c r="B58" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" ht="112.5">
-      <c r="A59" s="16"/>
-      <c r="B59" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
-      </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" ht="37.5">
+    <row r="60" spans="1:8" ht="93.75">
       <c r="A60" s="16"/>
       <c r="B60" s="2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="D60" s="2">
-        <v>2</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F60" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="G60" s="3" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="75">
       <c r="A61" s="16"/>
-      <c r="B61" s="2" t="s">
-        <v>115</v>
+      <c r="B61" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="D61" s="2">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="F61" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="G61" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="75">
+    <row r="62" spans="1:8" ht="112.5">
       <c r="A62" s="16"/>
       <c r="B62" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D62" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="F62" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="G62" s="3" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" ht="37.5">
       <c r="A63" s="16"/>
       <c r="B63" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="D63" s="2">
         <v>2</v>
       </c>
-      <c r="E63" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="E63" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+        <v>80</v>
+      </c>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" ht="75">
       <c r="A64" s="16"/>
       <c r="B64" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="D64" s="2">
-        <v>1</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
       <c r="G64" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+        <v>10</v>
+      </c>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="75">
       <c r="A65" s="16"/>
       <c r="B65" s="2" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="D65" s="2">
-        <v>2</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
       <c r="G65" s="3" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="16"/>
       <c r="B66" s="2" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>122</v>
+        <v>30</v>
       </c>
       <c r="D66" s="2">
-        <v>1</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="G66" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" ht="112.5">
+        <v>138</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="16"/>
       <c r="B67" s="2" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="2"/>
+        <v>137</v>
+      </c>
+      <c r="F67" s="5"/>
       <c r="G67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" ht="75">
+        <v>137</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="16"/>
       <c r="B68" s="2" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>72</v>
+        <v>122</v>
       </c>
       <c r="D68" s="2">
-        <v>46</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F68" s="5"/>
       <c r="G68" s="3" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="75">
+    <row r="69" spans="1:8">
       <c r="A69" s="16"/>
       <c r="B69" s="2" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="D69" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F69" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="F69" s="5"/>
       <c r="G69" s="3" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="75">
+    <row r="70" spans="1:8" ht="112.5">
       <c r="A70" s="16"/>
       <c r="B70" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D70" s="2">
-        <v>5</v>
-      </c>
-      <c r="E70" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="F70" s="2"/>
       <c r="G70" s="3" t="s">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="56.25">
+    <row r="71" spans="1:8" ht="75">
       <c r="A71" s="16"/>
-      <c r="B71" s="4" t="s">
-        <v>45</v>
+      <c r="B71" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="D71" s="2">
-        <v>10</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>108</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" ht="75">
+      <c r="A72" s="16"/>
+      <c r="B72" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D72" s="2">
+        <v>6</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" ht="75">
+      <c r="A73" s="16"/>
+      <c r="B73" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" s="2">
+        <v>5</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" ht="56.25">
+      <c r="A74" s="16"/>
+      <c r="B74" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="2">
+        <v>10</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F74" s="2"/>
+      <c r="G74" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="1:8" ht="56.25">
-      <c r="A72" s="16"/>
-      <c r="B72" s="11" t="s">
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" ht="56.25">
+      <c r="A75" s="16"/>
+      <c r="B75" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C75" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D75" s="7">
         <v>7</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E75" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="F72" s="7"/>
-      <c r="G72" s="12" t="s">
+      <c r="F75" s="7"/>
+      <c r="G75" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="10"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
-      <c r="H73" s="10"/>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="15" t="s">
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B77" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C77" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="8">
-        <v>1</v>
-      </c>
-      <c r="E74" s="8" t="s">
+      <c r="D77" s="8">
+        <v>1</v>
+      </c>
+      <c r="E77" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8" t="s">
+      <c r="F77" s="8"/>
+      <c r="G77" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H74" s="8"/>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="16"/>
-      <c r="B75" s="2" t="s">
+      <c r="H77" s="8"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="16"/>
+      <c r="B78" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D75" s="2">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="3" t="s">
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+      <c r="E78" s="2"/>
+      <c r="F78" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="16"/>
-      <c r="B76" s="7" t="s">
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="16"/>
+      <c r="B79" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C79" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D79" s="7">
         <v>2</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E79" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12" t="s">
+      <c r="F79" s="12"/>
+      <c r="G79" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="H76" s="12" t="s">
+      <c r="H79" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="10"/>
-      <c r="B77" s="10"/>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10"/>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="16" t="s">
+    <row r="80" spans="1:8">
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B81" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C81" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D78" s="8">
-        <v>1</v>
-      </c>
-      <c r="E78" s="8" t="s">
+      <c r="D81" s="8">
+        <v>1</v>
+      </c>
+      <c r="E81" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8" t="s">
+      <c r="F81" s="8"/>
+      <c r="G81" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H78" s="8"/>
-    </row>
-    <row r="79" spans="1:8" ht="56.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D79" s="2">
-        <v>1</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H79" s="2"/>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="16"/>
-      <c r="B80" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2">
-        <v>1</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="1:8" ht="37.5">
-      <c r="A81" s="16"/>
-      <c r="B81" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D81" s="2">
-        <v>1</v>
-      </c>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
-      <c r="G81" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H81" s="2"/>
+      <c r="H81" s="8"/>
     </row>
     <row r="82" spans="1:8" ht="37.5">
       <c r="A82" s="16"/>
       <c r="B82" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="16"/>
       <c r="B83" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C83" s="2"/>
       <c r="D83" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="16"/>
       <c r="B84" s="2" t="s">
-        <v>110</v>
+        <v>18</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="D84" s="2">
         <v>1</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="16"/>
       <c r="B85" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>83</v>
+        <v>21</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="D85" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F85" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="F85" s="3"/>
       <c r="G85" s="3" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="16"/>
       <c r="B86" s="2" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D86" s="2">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" s="3"/>
       <c r="G86" s="3" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="16"/>
-      <c r="B87" s="2"/>
+      <c r="B87" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="C87" s="4" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="D87" s="2">
-        <v>2</v>
-      </c>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F87" s="3"/>
+      <c r="G87" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="16"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D88" s="7">
+      <c r="B88" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D88" s="2">
+        <v>4</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F88" s="2"/>
+      <c r="G88" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="16"/>
+      <c r="B89" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1</v>
+      </c>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="16"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" s="2">
         <v>2</v>
       </c>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="7"/>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="10"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="10"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="10"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
-      <c r="H89" s="10"/>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D90" s="8">
-        <v>1</v>
-      </c>
-      <c r="E90" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H90" s="8"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="2"/>
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="16"/>
-      <c r="B91" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D91" s="2">
-        <v>1</v>
-      </c>
-      <c r="E91" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="F91" s="19"/>
-      <c r="G91" s="19"/>
-      <c r="H91" s="20"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D91" s="7">
+        <v>2</v>
+      </c>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="7"/>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="16"/>
-      <c r="B92" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D92" s="2">
-        <v>1</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F92" s="2"/>
-      <c r="G92" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H92" s="2"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="16"/>
-      <c r="B93" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D93" s="2">
-        <v>1</v>
-      </c>
-      <c r="E93" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F93" s="19"/>
-      <c r="G93" s="19"/>
-      <c r="H93" s="20"/>
+      <c r="A93" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D93" s="8">
+        <v>1</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="16"/>
       <c r="B94" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="D94" s="2">
         <v>1</v>
       </c>
-      <c r="E94" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="F94" s="19"/>
-      <c r="G94" s="19"/>
-      <c r="H94" s="20"/>
+      <c r="E94" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F94" s="22"/>
+      <c r="G94" s="22"/>
+      <c r="H94" s="23"/>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="16"/>
       <c r="B95" s="2" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D95" s="2">
         <v>1</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H95" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="16"/>
       <c r="B96" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F96" s="22"/>
+      <c r="G96" s="22"/>
+      <c r="H96" s="23"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="16"/>
+      <c r="B97" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="23"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="16"/>
+      <c r="B98" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F98" s="2"/>
+      <c r="G98" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="16"/>
+      <c r="B99" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D96" s="2">
-        <v>1</v>
-      </c>
-      <c r="E96" s="3" t="s">
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="F96" s="2"/>
-      <c r="G96" s="3" t="s">
+      <c r="F99" s="2"/>
+      <c r="G99" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="17"/>
-      <c r="B97" s="13" t="s">
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="17"/>
+      <c r="B100" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C97" s="13" t="s">
+      <c r="C100" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D97" s="13">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="s">
+      <c r="D100" s="13">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2" t="s">
+      <c r="F100" s="2"/>
+      <c r="G100" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H97" s="2"/>
+      <c r="H100" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="B2:H16">
-    <sortCondition ref="B2:B16"/>
+  <sortState ref="B44:H49">
+    <sortCondition ref="B44:B49"/>
   </sortState>
-  <mergeCells count="14">
-    <mergeCell ref="A47:A54"/>
+  <mergeCells count="15">
+    <mergeCell ref="A59:A75"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A81:A91"/>
+    <mergeCell ref="A93:A100"/>
+    <mergeCell ref="E97:H97"/>
+    <mergeCell ref="E96:H96"/>
+    <mergeCell ref="E94:H94"/>
+    <mergeCell ref="A50:A57"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A26"/>
     <mergeCell ref="A34:A38"/>
-    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A44:A49"/>
     <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A56:A72"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A78:A88"/>
-    <mergeCell ref="A90:A97"/>
-    <mergeCell ref="E94:H94"/>
-    <mergeCell ref="E93:H93"/>
-    <mergeCell ref="E91:H91"/>
+    <mergeCell ref="A41:A43"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="E56" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G56" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G76" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E76" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G57" r:id="rId5" location="prettyphoto/0/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G61" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G62" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G79" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E79" r:id="rId9" display="SeedStudio" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G80" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E80" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G81" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E82" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E84" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G84" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G67" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E67" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E85" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G85" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G86" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G68" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G69" r:id="rId22" display="wilco" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G70" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G71" r:id="rId24" display="wilco" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G72" r:id="rId25" display="wilco" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G59" r:id="rId26" location="prettyphoto/83/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G58" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G92" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E95" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H95" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H56" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F56" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G75" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F75" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F59" r:id="rId35" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType=" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F58" r:id="rId36" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType=" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F57" r:id="rId37" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType=" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="G60" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E60" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="G82" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="E83" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="E69" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E63" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="F63" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="H63" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="E91" r:id="rId46" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="E93" r:id="rId47" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="E92" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E71" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="E72" r:id="rId50" display="Hirosugi-Keiki(SRU-2010)" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="G96" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="E96" r:id="rId52" display="Amaaon" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="G65" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="G66" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E65" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="E66" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="H64" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="G95" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="G83" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="H76" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="G64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="E64" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="G63" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="E94" r:id="rId64" display="Seeed" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="F93" r:id="rId65" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="G93" r:id="rId66" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="H93" r:id="rId67" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="F91" r:id="rId68" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="G91" r:id="rId69" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="H91" r:id="rId70" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E59" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G59" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G79" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E79" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G60" r:id="rId5" location="prettyphoto/0/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G64" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G65" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G82" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E82" r:id="rId9" display="SeedStudio" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G83" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E83" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G84" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E85" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E87" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G87" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G70" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E70" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E88" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G88" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G89" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G71" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G72" r:id="rId22" display="wilco" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G73" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G74" r:id="rId24" display="wilco" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G75" r:id="rId25" display="wilco" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G62" r:id="rId26" location="prettyphoto/83/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G61" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G95" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E98" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H98" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H59" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F59" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G78" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F78" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F62" r:id="rId35" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType=" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F61" r:id="rId36" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType=" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F60" r:id="rId37" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType=" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G63" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E63" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="G85" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E86" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E72" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E66" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F66" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H66" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E94" r:id="rId46" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E96" r:id="rId47" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E95" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E74" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E75" r:id="rId50" display="Hirosugi-Keiki(SRU-2010)" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="G99" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E99" r:id="rId52" display="Amaaon" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G68" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G69" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E68" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E69" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H67" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G98" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G86" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H79" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G67" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E67" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="E97" r:id="rId64" display="Seeed" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F96" r:id="rId65" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G96" r:id="rId66" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="H96" r:id="rId67" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F94" r:id="rId68" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G94" r:id="rId69" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="H94" r:id="rId70" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" r:id="rId71"/>

</xml_diff>

<commit_message>
fix hyper link for DCDC converter
</commit_message>
<xml_diff>
--- a/HACKberry_BOM_v2.xlsx
+++ b/HACKberry_BOM_v2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_3F3A2CF4A0F6596A2FCAA4E82B699D9BFCB48192" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{095899E0-EE3E-4EDA-AD81-897B84E48CD0}"/>
   <bookViews>
-    <workbookView xWindow="-6000" yWindow="-21135" windowWidth="38400" windowHeight="21135" tabRatio="589" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6000" yWindow="-21132" windowWidth="38400" windowHeight="21132" tabRatio="589" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Full kit" sheetId="1" r:id="rId1"/>
@@ -12,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Full kit'!$A$1:$H$100</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="257">
   <si>
     <t>Part Name</t>
     <phoneticPr fontId="1"/>
@@ -269,10 +270,6 @@
 -Free Angle:270
 -Active coil turns:5
 -Arm length:12</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sotec</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1252,7 +1249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1276,6 +1273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1285,6 +1283,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1293,15 +1300,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1611,24 +1609,24 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.75" customWidth="1"/>
-    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1640,27 +1638,27 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="15" t="s">
-        <v>130</v>
+      <c r="A2" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -1671,12 +1669,12 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="16"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -1687,12 +1685,12 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="16"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -1703,12 +1701,12 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="16"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -1719,12 +1717,12 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1735,12 +1733,12 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1751,12 +1749,12 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -1767,12 +1765,12 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -1783,12 +1781,12 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -1799,12 +1797,12 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -1815,12 +1813,12 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="16"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1831,12 +1829,12 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -1847,12 +1845,12 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="16"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -1863,12 +1861,12 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -1879,12 +1877,12 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
@@ -1895,14 +1893,14 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="15" t="s">
-        <v>129</v>
+      <c r="A17" s="16" t="s">
+        <v>128</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D17" s="2">
         <v>1</v>
@@ -1913,12 +1911,12 @@
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -1929,12 +1927,12 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -1945,12 +1943,12 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -1961,12 +1959,12 @@
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="16"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -1977,12 +1975,12 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" s="2">
         <v>1</v>
@@ -1993,12 +1991,12 @@
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D23" s="2">
         <v>1</v>
@@ -2009,12 +2007,12 @@
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D24" s="2">
         <v>1</v>
@@ -2025,12 +2023,12 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
@@ -2041,12 +2039,12 @@
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="17"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -2057,14 +2055,14 @@
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="15" t="s">
-        <v>128</v>
+      <c r="A27" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -2075,12 +2073,12 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="16"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D28" s="2">
         <v>1</v>
@@ -2091,12 +2089,12 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="16"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -2107,12 +2105,12 @@
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="16"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="2">
         <v>1</v>
@@ -2123,12 +2121,12 @@
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -2139,12 +2137,12 @@
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="16"/>
+      <c r="A32" s="17"/>
       <c r="B32" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
@@ -2155,12 +2153,12 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="16"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D33" s="2">
         <v>1</v>
@@ -2171,14 +2169,14 @@
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="18" t="s">
-        <v>86</v>
+      <c r="A34" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
@@ -2189,12 +2187,12 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="19"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D35" s="2">
         <v>3</v>
@@ -2205,12 +2203,12 @@
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="19"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D36" s="2">
         <v>3</v>
@@ -2221,12 +2219,12 @@
       <c r="H36" s="2"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="19"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D37" s="2">
         <v>3</v>
@@ -2237,12 +2235,12 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="20"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D38" s="2">
         <v>3</v>
@@ -2253,14 +2251,14 @@
       <c r="H38" s="2"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="15" t="s">
-        <v>131</v>
+      <c r="A39" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D39" s="2">
         <v>1</v>
@@ -2271,12 +2269,12 @@
       <c r="H39" s="2"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="17"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D40" s="2">
         <v>1</v>
@@ -2287,14 +2285,14 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -2305,12 +2303,12 @@
       <c r="H41" s="2"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -2321,12 +2319,12 @@
       <c r="H42" s="2"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="17"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
@@ -2337,14 +2335,14 @@
       <c r="H43" s="2"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="15" t="s">
-        <v>132</v>
+      <c r="A44" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D44" s="2">
         <v>1</v>
@@ -2355,12 +2353,12 @@
       <c r="H44" s="2"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="16"/>
+      <c r="A45" s="17"/>
       <c r="B45" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D45" s="2">
         <v>1</v>
@@ -2371,12 +2369,12 @@
       <c r="H45" s="2"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D46" s="2">
         <v>1</v>
@@ -2387,12 +2385,12 @@
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="16"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D47" s="2">
         <v>1</v>
@@ -2403,12 +2401,12 @@
       <c r="H47" s="2"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="16"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D48" s="2">
         <v>1</v>
@@ -2419,12 +2417,12 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="17"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
@@ -2435,14 +2433,14 @@
       <c r="H49" s="2"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="15" t="s">
-        <v>133</v>
+      <c r="A50" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D50" s="2">
         <v>1</v>
@@ -2453,12 +2451,12 @@
       <c r="H50" s="2"/>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="16"/>
+      <c r="A51" s="17"/>
       <c r="B51" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D51" s="2">
         <v>1</v>
@@ -2469,12 +2467,12 @@
       <c r="H51" s="2"/>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="16"/>
+      <c r="A52" s="17"/>
       <c r="B52" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
@@ -2485,12 +2483,12 @@
       <c r="H52" s="2"/>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="16"/>
+      <c r="A53" s="17"/>
       <c r="B53" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
@@ -2501,12 +2499,12 @@
       <c r="H53" s="2"/>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="16"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
@@ -2517,12 +2515,12 @@
       <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="16"/>
+      <c r="A55" s="17"/>
       <c r="B55" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D55" s="2">
         <v>1</v>
@@ -2533,12 +2531,12 @@
       <c r="H55" s="2"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="16"/>
+      <c r="A56" s="17"/>
       <c r="B56" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D56" s="2">
         <v>1</v>
@@ -2549,12 +2547,12 @@
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="16"/>
+      <c r="A57" s="17"/>
       <c r="B57" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D57" s="7">
         <v>1</v>
@@ -2575,14 +2573,14 @@
       <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="15" t="s">
-        <v>60</v>
+      <c r="A59" s="16" t="s">
+        <v>59</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" s="8">
         <v>1</v>
@@ -2591,19 +2589,19 @@
         <v>4</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="93.75">
-      <c r="A60" s="16"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="90">
+      <c r="A60" s="17"/>
       <c r="B60" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
@@ -2613,35 +2611,35 @@
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="75">
-      <c r="A61" s="16"/>
+    <row r="61" spans="1:8" ht="72">
+      <c r="A61" s="17"/>
       <c r="B61" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="112.5">
-      <c r="A62" s="16"/>
+    <row r="62" spans="1:8" ht="108">
+      <c r="A62" s="17"/>
       <c r="B62" s="2" t="s">
         <v>52</v>
       </c>
@@ -2653,17 +2651,17 @@
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="36">
+      <c r="A63" s="17"/>
+      <c r="B63" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="1:8" ht="37.5">
-      <c r="A63" s="16"/>
-      <c r="B63" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>51</v>
@@ -2672,21 +2670,21 @@
         <v>2</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="75">
-      <c r="A64" s="16"/>
+    <row r="64" spans="1:8" ht="72">
+      <c r="A64" s="17"/>
       <c r="B64" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D64" s="2">
         <v>25</v>
@@ -2698,8 +2696,8 @@
       </c>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="75">
-      <c r="A65" s="16"/>
+    <row r="65" spans="1:8" ht="72">
+      <c r="A65" s="17"/>
       <c r="B65" s="2" t="s">
         <v>11</v>
       </c>
@@ -2717,9 +2715,9 @@
       <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="16"/>
+      <c r="A66" s="17"/>
       <c r="B66" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>30</v>
@@ -2728,22 +2726,22 @@
         <v>2</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="16"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>31</v>
@@ -2752,58 +2750,58 @@
         <v>1</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="16"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D68" s="2">
         <v>2</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="16"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="112.5">
-      <c r="A70" s="16"/>
+    <row r="70" spans="1:8" ht="108">
+      <c r="A70" s="17"/>
       <c r="B70" s="2" t="s">
         <v>32</v>
       </c>
@@ -2814,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="3" t="s">
@@ -2822,13 +2820,13 @@
       </c>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="75">
-      <c r="A71" s="16"/>
+    <row r="71" spans="1:8" ht="72">
+      <c r="A71" s="17"/>
       <c r="B71" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D71" s="2">
         <v>46</v>
@@ -2840,8 +2838,8 @@
       </c>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="75">
-      <c r="A72" s="16"/>
+    <row r="72" spans="1:8" ht="72">
+      <c r="A72" s="17"/>
       <c r="B72" s="2" t="s">
         <v>40</v>
       </c>
@@ -2852,7 +2850,7 @@
         <v>6</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="3" t="s">
@@ -2860,8 +2858,8 @@
       </c>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="75">
-      <c r="A73" s="16"/>
+    <row r="73" spans="1:8" ht="72">
+      <c r="A73" s="17"/>
       <c r="B73" s="2" t="s">
         <v>41</v>
       </c>
@@ -2874,12 +2872,12 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="56.25">
-      <c r="A74" s="16"/>
+    <row r="74" spans="1:8" ht="54">
+      <c r="A74" s="17"/>
       <c r="B74" s="4" t="s">
         <v>45</v>
       </c>
@@ -2890,7 +2888,7 @@
         <v>10</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="3" t="s">
@@ -2898,8 +2896,8 @@
       </c>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="56.25">
-      <c r="A75" s="16"/>
+    <row r="75" spans="1:8" ht="54">
+      <c r="A75" s="17"/>
       <c r="B75" s="11" t="s">
         <v>46</v>
       </c>
@@ -2910,7 +2908,7 @@
         <v>7</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="12" t="s">
@@ -2929,8 +2927,8 @@
       <c r="H76" s="10"/>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="15" t="s">
-        <v>135</v>
+      <c r="A77" s="16" t="s">
+        <v>134</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>6</v>
@@ -2942,28 +2940,28 @@
         <v>1</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F77" s="8"/>
       <c r="G77" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H77" s="8"/>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="16"/>
+      <c r="A78" s="17"/>
       <c r="B78" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D78" s="2">
         <v>1</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>28</v>
@@ -2971,25 +2969,25 @@
       <c r="H78" s="2"/>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="16"/>
+      <c r="A79" s="17"/>
       <c r="B79" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C79" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="D79" s="7">
         <v>2</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F79" s="12"/>
       <c r="G79" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H79" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3003,8 +3001,8 @@
       <c r="H80" s="10"/>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="16" t="s">
-        <v>134</v>
+      <c r="A81" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>23</v>
@@ -3016,36 +3014,36 @@
         <v>1</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H81" s="8"/>
     </row>
-    <row r="82" spans="1:8" ht="37.5">
-      <c r="A82" s="16"/>
+    <row r="82" spans="1:8" ht="36">
+      <c r="A82" s="17"/>
       <c r="B82" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D82" s="2">
         <v>1</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F82" s="3"/>
-      <c r="G82" s="3" t="s">
+      <c r="G82" s="15" t="s">
         <v>14</v>
       </c>
       <c r="H82" s="2"/>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="16"/>
+      <c r="A83" s="17"/>
       <c r="B83" s="2" t="s">
         <v>15</v>
       </c>
@@ -3063,7 +3061,7 @@
       <c r="H83" s="2"/>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="16"/>
+      <c r="A84" s="17"/>
       <c r="B84" s="2" t="s">
         <v>18</v>
       </c>
@@ -3081,12 +3079,12 @@
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="16"/>
+      <c r="A85" s="17"/>
       <c r="B85" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D85" s="2">
         <v>1</v>
@@ -3096,14 +3094,14 @@
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="16"/>
+      <c r="A86" s="17"/>
       <c r="B86" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>25</v>
@@ -3116,17 +3114,17 @@
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="16"/>
+      <c r="A87" s="17"/>
       <c r="B87" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D87" s="2">
         <v>1</v>
@@ -3141,12 +3139,12 @@
       <c r="H87" s="2"/>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="16"/>
+      <c r="A88" s="17"/>
       <c r="B88" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D88" s="2">
         <v>4</v>
@@ -3161,12 +3159,12 @@
       <c r="H88" s="2"/>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="16"/>
+      <c r="A89" s="17"/>
       <c r="B89" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
@@ -3179,10 +3177,10 @@
       <c r="H89" s="2"/>
     </row>
     <row r="90" spans="1:8">
-      <c r="A90" s="16"/>
+      <c r="A90" s="17"/>
       <c r="B90" s="2"/>
       <c r="C90" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D90" s="2">
         <v>2</v>
@@ -3193,10 +3191,10 @@
       <c r="H90" s="2"/>
     </row>
     <row r="91" spans="1:8">
-      <c r="A91" s="16"/>
+      <c r="A91" s="17"/>
       <c r="B91" s="7"/>
       <c r="C91" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D91" s="7">
         <v>2</v>
@@ -3217,160 +3215,160 @@
       <c r="H92" s="10"/>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="16" t="s">
-        <v>127</v>
+      <c r="A93" s="17" t="s">
+        <v>126</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C93" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C93" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="D93" s="8">
         <v>1</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F93" s="8"/>
       <c r="G93" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H93" s="8"/>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="16"/>
+      <c r="A94" s="17"/>
       <c r="B94" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C94" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="D94" s="2">
         <v>1</v>
       </c>
-      <c r="E94" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="F94" s="22"/>
-      <c r="G94" s="22"/>
-      <c r="H94" s="23"/>
+      <c r="E94" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="21"/>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" s="16"/>
+      <c r="A95" s="17"/>
       <c r="B95" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
+      <c r="E95" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D95" s="2">
-        <v>1</v>
-      </c>
-      <c r="E95" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H95" s="2"/>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="16"/>
+      <c r="A96" s="17"/>
       <c r="B96" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20"/>
+      <c r="H96" s="21"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="17"/>
+      <c r="B97" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D96" s="2">
-        <v>1</v>
-      </c>
-      <c r="E96" s="21" t="s">
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+      <c r="E97" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="23"/>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="16"/>
-      <c r="B97" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D97" s="2">
-        <v>1</v>
-      </c>
-      <c r="E97" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F97" s="22"/>
-      <c r="G97" s="22"/>
-      <c r="H97" s="23"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+      <c r="H97" s="21"/>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="16"/>
+      <c r="A98" s="17"/>
       <c r="B98" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D98" s="2">
         <v>1</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="17"/>
+      <c r="B99" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="H98" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
-      <c r="A99" s="16"/>
-      <c r="B99" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D99" s="2">
-        <v>1</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H99" s="2"/>
     </row>
     <row r="100" spans="1:8">
-      <c r="A100" s="17"/>
+      <c r="A100" s="18"/>
       <c r="B100" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D100" s="13">
+        <v>1</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="D100" s="13">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H100" s="2"/>
     </row>
@@ -3379,13 +3377,6 @@
     <sortCondition ref="B44:B49"/>
   </sortState>
   <mergeCells count="15">
-    <mergeCell ref="A59:A75"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="A81:A91"/>
-    <mergeCell ref="A93:A100"/>
-    <mergeCell ref="E97:H97"/>
-    <mergeCell ref="E96:H96"/>
-    <mergeCell ref="E94:H94"/>
     <mergeCell ref="A50:A57"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="A2:A16"/>
@@ -3394,6 +3385,13 @@
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A59:A75"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A81:A91"/>
+    <mergeCell ref="A93:A100"/>
+    <mergeCell ref="E97:H97"/>
+    <mergeCell ref="E96:H96"/>
+    <mergeCell ref="E94:H94"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -3404,69 +3402,69 @@
     <hyperlink ref="G60" r:id="rId5" location="prettyphoto/0/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="G64" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="G65" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G82" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E82" r:id="rId9" display="SeedStudio" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G83" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E83" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G84" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E85" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E87" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G87" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G70" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E70" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E88" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G88" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G89" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G71" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G72" r:id="rId22" display="wilco" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G73" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G74" r:id="rId24" display="wilco" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G75" r:id="rId25" display="wilco" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="G62" r:id="rId26" location="prettyphoto/83/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G61" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G95" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E98" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H98" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H59" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F59" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="G78" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F78" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F62" r:id="rId35" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType=" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F61" r:id="rId36" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType=" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F60" r:id="rId37" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType=" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="G63" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E63" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="G85" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="E86" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="E72" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E66" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="F66" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="H66" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="E94" r:id="rId46" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="E96" r:id="rId47" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="E95" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E74" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="E75" r:id="rId50" display="Hirosugi-Keiki(SRU-2010)" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="G99" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="E99" r:id="rId52" display="Amaaon" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="G68" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="G69" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E68" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="E69" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="H67" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="G98" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="G86" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="H79" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="G67" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="E67" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="G66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="E97" r:id="rId64" display="Seeed" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="F96" r:id="rId65" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="G96" r:id="rId66" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="H96" r:id="rId67" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="F94" r:id="rId68" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="G94" r:id="rId69" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="H94" r:id="rId70" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E82" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G83" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E83" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G84" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E85" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E87" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G87" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G70" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E70" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E88" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G88" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G89" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G71" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G72" r:id="rId21" display="wilco" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G73" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G74" r:id="rId23" display="wilco" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G75" r:id="rId24" display="wilco" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G62" r:id="rId25" location="prettyphoto/83/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G61" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G95" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E98" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H98" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H59" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F59" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G78" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F78" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F62" r:id="rId34" display="http://www.leespring.com/product_spec.asp?partnum=LTL012A05M&amp;springType=T&amp;subType=" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F61" r:id="rId35" display="http://www.leespring.com/product_spec.asp?partnum=LE014A02S&amp;springType=E&amp;subType=" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F60" r:id="rId36" display="http://www.leespring.com/product_spec.asp?partnum=LCM050C02M&amp;springType=C&amp;subType=" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="G63" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E63" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="G85" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="E86" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E72" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E66" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F66" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H66" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E94" r:id="rId45" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="E96" r:id="rId46" display="Seeed" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E95" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E74" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E75" r:id="rId49" display="Hirosugi-Keiki(SRU-2010)" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="G99" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="E99" r:id="rId51" display="Amaaon" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="G68" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G69" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E68" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E69" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H67" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="G98" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="G86" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="H79" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="G67" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E67" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="G66" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="E97" r:id="rId63" display="Seeed" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F96" r:id="rId64" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="G96" r:id="rId65" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="H96" r:id="rId66" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F94" r:id="rId67" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="G94" r:id="rId68" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="H94" r:id="rId69" display="https://www.seeedstudio.com/opl.html" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="G82" r:id="rId70" xr:uid="{110FB737-B04C-4B5D-AA77-D62256EDFB45}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="4294967293" r:id="rId71"/>

</xml_diff>